<commit_message>
Refactor Chapter 3: Improve clarity and structure of threat modeling discussion
- Enhanced readability by adjusting sentence structures and removing redundant phrases.
- Updated references and page numbers in the bibliography and table of contents.
- Revised draft date in the document header to reflect the new submission timeline.
- Removed unnecessary sections and streamlined content for better flow.
- Corrected minor typographical errors and improved consistency in terminology.
</commit_message>
<xml_diff>
--- a/References/Gantt.xlsx
+++ b/References/Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D588897-10E2-463E-AAC3-927301B36BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1E5625-6FD4-46DE-8B83-F155CA14019E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11865" yWindow="2715" windowWidth="19200" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planeador de Projetos" sheetId="1" r:id="rId1"/>
@@ -935,7 +935,7 @@
   <dimension ref="B1:BO30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -970,7 +970,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="14">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="24" t="s">

</xml_diff>